<commit_message>
Finalizacion de Relacion Tramites
</commit_message>
<xml_diff>
--- a/Docs/RelacionTramites.xlsx
+++ b/Docs/RelacionTramites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\lap\Git\Iciplaam\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA1F783-9379-4D0C-87D8-5F7CCB31B50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8136B304-8A64-46C3-A7E9-0DF6A34D4BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{A071996E-BB0B-4A49-9270-7ED025398E09}"/>
   </bookViews>
@@ -246,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -276,15 +276,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -602,46 +599,44 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
     <col min="15" max="15" width="13" customWidth="1"/>
     <col min="16" max="16" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
     </row>
     <row r="2" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="18" t="s">
-        <v>1</v>
-      </c>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="G2" s="18" t="s">
+        <v>1</v>
+      </c>
       <c r="I2" s="18"/>
       <c r="J2" s="18"/>
       <c r="K2" s="18"/>
@@ -652,24 +647,24 @@
       <c r="P2" s="18"/>
     </row>
     <row r="3" spans="1:16" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F4" s="1"/>
@@ -794,11 +789,6 @@
       <c r="P7" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A2:P2"/>
-    <mergeCell ref="A3:P3"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>